<commit_message>
Notebook 10 Exp series 1
</commit_message>
<xml_diff>
--- a/January 2023 Analysis/New Analysis/sampleset/Results/Result 10 Exp 10.xlsx
+++ b/January 2023 Analysis/New Analysis/sampleset/Results/Result 10 Exp 10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rashedhasan/Desktop/UNL/Research/Object relational mapping/Step 5 - Abstraction/OM-Solution_Mapping/OM-ML_Research/January 2023 Analysis/New Analysis/sampleset/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71391D95-2A46-8747-A1C9-4BA687A6FD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71CA45B-6ED1-BF4B-9D04-F46871792589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{9E606C90-6937-7643-AC22-ADE071A6A0E2}"/>
+    <workbookView xWindow="2320" yWindow="3540" windowWidth="28040" windowHeight="16380" xr2:uid="{9E606C90-6937-7643-AC22-ADE071A6A0E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,7 +345,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -370,6 +370,11 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
@@ -398,7 +403,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,7 +721,7 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A95" sqref="A1:A101"/>
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,462 +731,462 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="2"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="1"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="1"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="2"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="2"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="1"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="2"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B54" s="2"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B57" s="1"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B58" s="2"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B59" s="2"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B60" s="2"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B62" s="1"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B63" s="2"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B64" s="2"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B65" s="2"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B66" s="2"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B67" s="2"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B68" s="2"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B71" s="2"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B72" s="2"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B73" s="2"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B74" s="2"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B75" s="2"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B76" s="2"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B77" s="2"/>
@@ -1193,115 +1198,115 @@
       <c r="B78" s="1"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B79" s="2"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B80" s="2"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B81" s="2"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B84" s="2"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B85" s="2"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B86" s="2"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B87" s="2"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B88" s="1"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B89" s="2"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B90" s="2"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B91" s="2"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B92" s="2"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B93" s="2"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B94" s="2"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B95" s="2"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B96" s="2"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B97" s="2"/>
@@ -1313,19 +1318,19 @@
       <c r="B98" s="1"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
+      <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B99" s="2"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B100" s="2"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B101" s="2"/>

</xml_diff>